<commit_message>
Make test_read_waterlvl more complete
</commit_message>
<xml_diff>
--- a/gwhat/projet/tests/data/water_level_datafile.xlsx
+++ b/gwhat/projet/tests/data/water_level_datafile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\gwhat\gwhat\projet\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44E4D8F-58EF-4C1B-AE21-6A7D8093D485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96452F9D-0C52-4AA5-AE30-4594AEEDFC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>